<commit_message>
This is mainly a version that has a working slideshow however all the placeholders are in place for styling
</commit_message>
<xml_diff>
--- a/admin/writeups/Asset Table.xlsx
+++ b/admin/writeups/Asset Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DGM\Y13 digital media\Website\admin\writeups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6FDC81-9DAE-4859-88CD-B47DFEE0D6D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F03AFE-3598-46DA-974E-DEE4AB912921}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12225" xr2:uid="{38E3F455-74AF-42E9-83EF-7BA68CE6BE9C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>asset table</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>17KB</t>
+  </si>
+  <si>
+    <t>Aruld</t>
+  </si>
+  <si>
+    <t>BBC_Micro_Bit_with_original_Packaging.jpg</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:BBC_Micro_Bit_with_original_Packaging.jpg</t>
+  </si>
+  <si>
+    <t>4,527KB</t>
   </si>
 </sst>
 </file>
@@ -186,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -317,19 +329,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -372,7 +407,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -913,6 +954,67 @@
         <a:xfrm>
           <a:off x="228601" y="6924675"/>
           <a:ext cx="695324" cy="695324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>98428</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1038223</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>723896</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="https://upload.wikimedia.org/wikipedia/commons/c/cb/BBC_Micro_Bit_with_original_Packaging.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92B3E3B3-F2DD-454A-9364-BB36E16F95E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="98428" y="7229475"/>
+          <a:ext cx="939795" cy="704846"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1233,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DB3B30-C405-4D0D-8E61-81609B8D57C3}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,224 +1345,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+    <row r="12" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1472,9 +1586,10 @@
     <hyperlink ref="C9" r:id="rId6" xr:uid="{64F88A89-619D-4A09-A4C5-11205B42933E}"/>
     <hyperlink ref="C10" r:id="rId7" xr:uid="{EBEAFDD2-2052-44E2-9310-523821FAD2AC}"/>
     <hyperlink ref="C11" r:id="rId8" xr:uid="{EC71EAAE-D5BC-470E-B7FE-3A8942183F74}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{A0E99B1B-A9AC-47D8-B3FB-601FD904CC31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
-  <drawing r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>